<commit_message>
add an asset to list
</commit_message>
<xml_diff>
--- a/Unity3D Assets Coasts.xlsx
+++ b/Unity3D Assets Coasts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\NoRPG-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$I$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$I$25</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>https://www.assetstore.unity3d.com/en/#!/content/19826</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Summe</t>
+  </si>
+  <si>
+    <t>https://www.assetstore.unity3d.com/en/#!/content/45786</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,6 +351,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -663,21 +670,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I25"/>
+  <dimension ref="B1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="11" width="5.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
@@ -1086,35 +1093,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="8">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12" t="s">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="13">
-        <f>SUM(I3:I24)</f>
-        <v>215</v>
+      <c r="I26" s="13">
+        <f>SUM(I3:I25)</f>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1146,21 @@
       <sortCondition ref="I2:I24"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="I3:I24">
+  <conditionalFormatting sqref="I3:I23 I25">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4093C14E-3065-4950-A5D8-0C91B4ACCB23}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I25">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1132,7 +1169,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4093C14E-3065-4950-A5D8-0C91B4ACCB23}</x14:id>
+          <x14:id>{27FBA6FE-B4A8-4CB9-8964-F11684496BA6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1156,13 +1193,14 @@
     <hyperlink ref="B18" r:id="rId16" location="!/content/56822"/>
     <hyperlink ref="B15" r:id="rId17" location="!/content/58300"/>
     <hyperlink ref="B17" r:id="rId18" location="!/content/19973"/>
-    <hyperlink ref="B24" r:id="rId19" location="!/content/9312"/>
+    <hyperlink ref="B25" r:id="rId19" location="!/content/9312"/>
     <hyperlink ref="B22" r:id="rId20" location="!/content/49171"/>
     <hyperlink ref="B14" r:id="rId21" location="!/content/20054"/>
     <hyperlink ref="B10" r:id="rId22" location="!/content/66322"/>
+    <hyperlink ref="B24" r:id="rId23" location="!/content/45786"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1175,7 +1213,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I3:I24</xm:sqref>
+          <xm:sqref>I3:I23 I25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{27FBA6FE-B4A8-4CB9-8964-F11684496BA6}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I3:I25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>